<commit_message>
Update data from UGent
</commit_message>
<xml_diff>
--- a/ugent.xlsx
+++ b/ugent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pheyvaer/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{141EFB5F-0728-B749-80CD-80E7995716AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23643AE-B525-7A41-9300-EE1F46E7A0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{352FD9BC-1EAA-024D-A361-6FAED15EC212}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>This is the data filled in by UGent, based on the template.</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -410,9 +413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70698F6A-2977-0A41-96FE-1E1FFB74B052}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -421,6 +426,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>